<commit_message>
First working version of the core functionality: - get board - get player index - get player moves - make moves
</commit_message>
<xml_diff>
--- a/BlokeeAutomation/Data/Config.xlsx
+++ b/BlokeeAutomation/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Hackaton\BlokeeAutomation\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath\Projects\Hackaton\Code\BlokeeAutomation\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCDF8022-8D99-4118-9A5C-58E2E0DB39D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2135D07-96F7-47FC-BC85-7A70481F940E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1615,7 +1615,7 @@
   <dimension ref="A1:Z992"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1762,7 +1762,7 @@
         <v>41</v>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
@@ -1770,7 +1770,7 @@
         <v>42</v>
       </c>
       <c r="B16">
-        <v>250</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1"/>

</xml_diff>